<commit_message>
updated inventory take detergentA and cleaning solution
</commit_message>
<xml_diff>
--- a/MMCCCL_supply_july.xlsx
+++ b/MMCCCL_supply_july.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vetdd\Documents\PostGrad_NSS\MMCCCL_supply\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBCFCFCF-DBE6-44CD-879B-1953678858C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46950492-51A2-4F7B-B07E-B801E5EC9340}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="720" windowWidth="23040" windowHeight="12228" xr2:uid="{16E4F072-8648-485F-BEC5-19999D3A63FC}"/>
   </bookViews>
@@ -1958,74 +1958,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -2042,10 +1974,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="FFFFFF"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="202020"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="0E2841"/>
@@ -2356,8 +2288,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94F06BF6-FE2E-478D-9CAE-09F3C98E411A}">
   <dimension ref="A1:K186"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A167" workbookViewId="0">
-      <selection activeCell="C184" sqref="C184"/>
+    <sheetView tabSelected="1" topLeftCell="A86" workbookViewId="0">
+      <selection activeCell="H95" sqref="H95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4032,7 +3964,7 @@
         <v>66</v>
       </c>
       <c r="H51" s="9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I51" s="6" t="s">
         <v>4</v>
@@ -5464,7 +5396,7 @@
         <v>66</v>
       </c>
       <c r="H95" s="12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I95" s="6" t="s">
         <v>44</v>

</xml_diff>

<commit_message>
add alert for reaching minimum reorder theshold
</commit_message>
<xml_diff>
--- a/MMCCCL_supply_july.xlsx
+++ b/MMCCCL_supply_july.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vetdd\Documents\PostGrad_NSS\MMCCCL_supply\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46950492-51A2-4F7B-B07E-B801E5EC9340}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D578C8A8-4544-4DA3-AE4E-F8BE2DDD2A45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="720" windowWidth="23040" windowHeight="12228" xr2:uid="{16E4F072-8648-485F-BEC5-19999D3A63FC}"/>
   </bookViews>
@@ -1624,9 +1624,6 @@
     <t xml:space="preserve">Uric Acid 2 </t>
   </si>
   <si>
-    <t>1 mL Syringe (unit = bag: 4 syringes per bag)</t>
-  </si>
-  <si>
     <r>
       <t>1000 ul Researh Barrier Tip</t>
     </r>
@@ -1791,6 +1788,9 @@
   </si>
   <si>
     <t>Urea Nitrogen Reagent (unit = cartridge: 400 reactions per cartridge)</t>
+  </si>
+  <si>
+    <t>1 mL Syringe (unit = each  syringe)</t>
   </si>
 </sst>
 </file>
@@ -2288,8 +2288,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94F06BF6-FE2E-478D-9CAE-09F3C98E411A}">
   <dimension ref="A1:K186"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A86" workbookViewId="0">
-      <selection activeCell="H95" sqref="H95"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H79" sqref="H79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2312,7 +2312,7 @@
         <v>397</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="D1" s="10" t="s">
         <v>395</v>
@@ -2344,7 +2344,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>525</v>
+        <v>574</v>
       </c>
       <c r="C2" s="5">
         <v>4</v>
@@ -2356,7 +2356,7 @@
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
       <c r="H2" s="12">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="I2" s="6" t="s">
         <v>44</v>
@@ -2373,7 +2373,7 @@
         <v>372</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="C3" s="5">
         <v>3</v>
@@ -2406,7 +2406,7 @@
         <v>20</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="C4" s="5">
         <v>1</v>
@@ -2501,7 +2501,7 @@
         <v>0</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="C7" s="5">
         <v>5</v>
@@ -2536,7 +2536,7 @@
         <v>0</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="6" t="s">
@@ -2569,7 +2569,7 @@
         <v>0</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="6" t="s">
@@ -2602,7 +2602,7 @@
         <v>0</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="C10" s="5">
         <v>2</v>
@@ -2637,7 +2637,7 @@
         <v>0</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="6" t="s">
@@ -2670,7 +2670,7 @@
         <v>0</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="C12" s="5">
         <v>2</v>
@@ -2705,7 +2705,7 @@
         <v>0</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="6" t="s">
@@ -2738,7 +2738,7 @@
         <v>20</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C14" s="1">
         <v>8</v>
@@ -2761,7 +2761,7 @@
       </c>
       <c r="J14" s="2"/>
       <c r="K14" s="20" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
@@ -2769,7 +2769,7 @@
         <v>0</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="C15" s="5">
         <v>2</v>
@@ -2804,7 +2804,7 @@
         <v>0</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="6" t="s">
@@ -2837,7 +2837,7 @@
         <v>0</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="6" t="s">
@@ -2870,7 +2870,7 @@
         <v>20</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="C18" s="5">
         <v>2</v>
@@ -2905,7 +2905,7 @@
         <v>20</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="6" t="s">
@@ -2938,7 +2938,7 @@
         <v>20</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="C20" s="5">
         <v>1</v>
@@ -2973,7 +2973,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="C21" s="5"/>
       <c r="D21" s="6" t="s">
@@ -3006,7 +3006,7 @@
         <v>0</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="C22" s="5">
         <v>1</v>
@@ -3041,7 +3041,7 @@
         <v>0</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="C23" s="5">
         <v>1</v>
@@ -3076,7 +3076,7 @@
         <v>20</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="C24" s="5">
         <v>1</v>
@@ -3144,7 +3144,7 @@
         <v>20</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="C26" s="5">
         <v>1</v>
@@ -3202,7 +3202,7 @@
         <v>20</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="C28" s="5">
         <v>2</v>
@@ -3272,7 +3272,7 @@
         <v>20</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="C30" s="5">
         <v>1</v>
@@ -3335,7 +3335,7 @@
         <v>20</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="C32" s="5">
         <v>1</v>
@@ -3401,7 +3401,7 @@
         <v>0</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C34" s="5">
         <v>2</v>
@@ -3436,7 +3436,7 @@
         <v>0</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C35" s="5"/>
       <c r="D35" s="6" t="s">
@@ -3504,7 +3504,7 @@
         <v>20</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C37" s="5">
         <v>1</v>
@@ -3533,7 +3533,7 @@
         <v>20</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C38" s="5"/>
       <c r="D38" s="6" t="s">
@@ -3566,7 +3566,7 @@
         <v>20</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="C39" s="5">
         <v>2</v>
@@ -3669,7 +3669,7 @@
         <v>346</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="C42" s="5">
         <v>5</v>
@@ -3692,7 +3692,7 @@
         <v>346</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="C43" s="5"/>
       <c r="D43" s="6" t="s">
@@ -3719,7 +3719,7 @@
         <v>0</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="C44" s="5">
         <v>5</v>
@@ -3754,7 +3754,7 @@
         <v>0</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="C45" s="5"/>
       <c r="D45" s="6" t="s">
@@ -3787,7 +3787,7 @@
         <v>20</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="C46" s="5">
         <v>5</v>
@@ -4144,7 +4144,7 @@
         <v>56</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="C57" s="5">
         <v>1</v>
@@ -4214,7 +4214,7 @@
         <v>88</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="C59" s="5">
         <v>1</v>
@@ -4284,7 +4284,7 @@
         <v>20</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="C61" s="5">
         <v>1</v>
@@ -4538,7 +4538,7 @@
         <v>20</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="C69" s="5">
         <v>1</v>
@@ -4571,7 +4571,7 @@
         <v>20</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="C70" s="5"/>
       <c r="D70" s="6" t="s">
@@ -4602,7 +4602,7 @@
         <v>0</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="C71" s="5">
         <v>1</v>
@@ -4769,7 +4769,7 @@
         <v>20</v>
       </c>
       <c r="B76" s="5" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="C76" s="5">
         <v>1</v>
@@ -4878,7 +4878,7 @@
         <v>249</v>
       </c>
       <c r="H79" s="12">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I79" s="6" t="s">
         <v>44</v>
@@ -5242,7 +5242,7 @@
         <v>0</v>
       </c>
       <c r="B91" s="5" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="C91" s="5">
         <v>5</v>
@@ -5448,7 +5448,7 @@
         <v>0</v>
       </c>
       <c r="B97" s="5" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="C97" s="5">
         <v>1</v>
@@ -5483,7 +5483,7 @@
         <v>0</v>
       </c>
       <c r="B98" s="5" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="C98" s="5"/>
       <c r="D98" s="6" t="s">
@@ -6743,7 +6743,7 @@
         <v>143</v>
       </c>
       <c r="B139" s="5" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="C139" s="5">
         <v>2</v>
@@ -6774,7 +6774,7 @@
         <v>389</v>
       </c>
       <c r="B140" s="5" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="C140" s="5"/>
       <c r="D140" s="6" t="s">
@@ -6894,7 +6894,7 @@
         <v>346</v>
       </c>
       <c r="B144" s="15" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="C144" s="15">
         <v>1</v>
@@ -6927,7 +6927,7 @@
         <v>346</v>
       </c>
       <c r="B145" s="15" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="C145" s="15">
         <v>1</v>
@@ -7049,7 +7049,7 @@
         <v>346</v>
       </c>
       <c r="B149" s="15" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="C149" s="15"/>
       <c r="D149" s="6" t="s">
@@ -7078,7 +7078,7 @@
         <v>346</v>
       </c>
       <c r="B150" s="15" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="C150" s="15"/>
       <c r="D150" s="6" t="s">
@@ -7175,7 +7175,7 @@
         <v>0</v>
       </c>
       <c r="B153" s="5" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="C153" s="5">
         <v>1</v>
@@ -7245,7 +7245,7 @@
         <v>0</v>
       </c>
       <c r="B155" s="5" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="C155" s="5">
         <v>2</v>
@@ -7278,7 +7278,7 @@
         <v>0</v>
       </c>
       <c r="B156" s="5" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="C156" s="5"/>
       <c r="D156" s="6" t="s">
@@ -7346,7 +7346,7 @@
         <v>20</v>
       </c>
       <c r="B158" s="5" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="C158" s="5">
         <v>1</v>
@@ -7484,7 +7484,7 @@
         <v>0</v>
       </c>
       <c r="B162" s="5" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="C162" s="5">
         <v>1</v>
@@ -7645,7 +7645,7 @@
         <v>346</v>
       </c>
       <c r="B167" s="5" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="C167" s="5">
         <v>2</v>
@@ -7674,7 +7674,7 @@
         <v>129</v>
       </c>
       <c r="B168" s="5" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C168" s="5">
         <v>5</v>
@@ -7709,7 +7709,7 @@
         <v>20</v>
       </c>
       <c r="B169" s="5" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="C169" s="5">
         <v>4</v>
@@ -7742,7 +7742,7 @@
         <v>20</v>
       </c>
       <c r="B170" s="5" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="C170" s="5"/>
       <c r="D170" s="6" t="s">
@@ -7841,7 +7841,7 @@
         <v>20</v>
       </c>
       <c r="B173" s="5" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="C173" s="5">
         <v>1</v>
@@ -7876,7 +7876,7 @@
         <v>20</v>
       </c>
       <c r="B174" s="5" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="C174" s="5"/>
       <c r="D174" s="6" t="s">
@@ -7907,7 +7907,7 @@
         <v>20</v>
       </c>
       <c r="B175" s="5" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="C175" s="5"/>
       <c r="D175" s="6" t="s">
@@ -7938,7 +7938,7 @@
         <v>261</v>
       </c>
       <c r="B176" s="5" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="C176" s="5">
         <v>2</v>
@@ -8002,7 +8002,7 @@
         <v>88</v>
       </c>
       <c r="B178" s="5" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="C178" s="5">
         <v>2</v>
@@ -8037,7 +8037,7 @@
         <v>104</v>
       </c>
       <c r="B179" s="5" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="C179" s="5"/>
       <c r="D179" s="6" t="s">
@@ -8070,7 +8070,7 @@
         <v>0</v>
       </c>
       <c r="B180" s="5" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="C180" s="5">
         <v>2</v>

</xml_diff>